<commit_message>
merge demographic data for big panel plot
</commit_message>
<xml_diff>
--- a/data/raw-data/SAA Ethics TF 2 Survey - 09-01-20 - Key.xlsx
+++ b/data/raw-data/SAA Ethics TF 2 Survey - 09-01-20 - Key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/saa-ethics-survey-2020/data/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38992E51-DB20-E74D-9CE2-6249D9C28AC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635ECEA9-23C9-2740-B136-D509B443882B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14140" yWindow="460" windowWidth="14660" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14140" yWindow="460" windowWidth="14660" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KEY" sheetId="6" r:id="rId1"/>
@@ -1276,7 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6CD661-9014-2F41-BED5-2598BED0F44C}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1505,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156328DD-468B-4E45-ABE4-AC9FF351BC96}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>